<commit_message>
criando o código ETL - Extract
</commit_message>
<xml_diff>
--- a/Database/dados-originais/uf-regioes-brasil/uf-regioes-brasil-siglas.xlsx
+++ b/Database/dados-originais/uf-regioes-brasil/uf-regioes-brasil-siglas.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e27a146a09249998/Área de Trabalho/WiseTour/Database/Dados Originais/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e27a146a09249998/Área de Trabalho/WiseTour/database/dados-originais/uf-regioes-brasil/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{BD884266-224B-4475-9D27-FD31DBB931D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{114B3BC8-4AE3-4590-ACE8-AACC737F2EF6}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="8_{BD884266-224B-4475-9D27-FD31DBB931D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9390C7C5-9D8D-4120-9BBB-7890BA3435CC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{874A780A-A36C-46BA-916D-F1942B0CCC0D}"/>
+    <workbookView minimized="1" xWindow="5124" yWindow="3708" windowWidth="17280" windowHeight="8880" xr2:uid="{874A780A-A36C-46BA-916D-F1942B0CCC0D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
+    <sheet name="Regiões" sheetId="3" r:id="rId1"/>
+    <sheet name="Unidades Federativas" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$2:$E$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Unidades Federativas'!$A$1:$C$28</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
   <si>
     <t>Rondônia</t>
   </si>
@@ -122,183 +123,105 @@
     <t>Sigla</t>
   </si>
   <si>
-    <t>Capital</t>
-  </si>
-  <si>
     <t>Região</t>
   </si>
   <si>
     <t>AC</t>
   </si>
   <si>
-    <t>Rio Branco</t>
-  </si>
-  <si>
     <t>Norte</t>
   </si>
   <si>
     <t>AL</t>
   </si>
   <si>
-    <t>Maceió</t>
-  </si>
-  <si>
     <t>Nordeste</t>
   </si>
   <si>
     <t>AP</t>
   </si>
   <si>
-    <t>Macapá</t>
-  </si>
-  <si>
     <t>AM</t>
   </si>
   <si>
-    <t>Manaus</t>
-  </si>
-  <si>
     <t>BA</t>
   </si>
   <si>
-    <t>Salvador</t>
-  </si>
-  <si>
     <t>CE</t>
   </si>
   <si>
-    <t>Fortaleza</t>
-  </si>
-  <si>
     <t>DF</t>
   </si>
   <si>
-    <t>Brasília</t>
-  </si>
-  <si>
     <t>Centro-Oeste</t>
   </si>
   <si>
     <t>ES</t>
   </si>
   <si>
-    <t>Vitória</t>
-  </si>
-  <si>
     <t>Sudeste</t>
   </si>
   <si>
     <t>GO</t>
   </si>
   <si>
-    <t>Goiânia</t>
-  </si>
-  <si>
     <t>MA</t>
   </si>
   <si>
-    <t>São Luís</t>
-  </si>
-  <si>
     <t>MT</t>
   </si>
   <si>
-    <t>Cuiabá</t>
-  </si>
-  <si>
     <t>MS</t>
   </si>
   <si>
-    <t>Campo Grande</t>
-  </si>
-  <si>
     <t>MG</t>
   </si>
   <si>
-    <t>Belo Horizonte</t>
-  </si>
-  <si>
     <t>PA</t>
   </si>
   <si>
-    <t>Belém</t>
-  </si>
-  <si>
     <t>PB</t>
   </si>
   <si>
-    <t>João Pessoa</t>
-  </si>
-  <si>
     <t>PR</t>
   </si>
   <si>
-    <t>Curitiba</t>
-  </si>
-  <si>
     <t>Sul</t>
   </si>
   <si>
     <t>PE</t>
   </si>
   <si>
-    <t>Recife</t>
-  </si>
-  <si>
     <t>PI</t>
   </si>
   <si>
-    <t>Teresina</t>
-  </si>
-  <si>
     <t>RJ</t>
   </si>
   <si>
     <t>RN</t>
   </si>
   <si>
-    <t>Natal</t>
-  </si>
-  <si>
     <t>RS</t>
   </si>
   <si>
-    <t>Porto Alegre</t>
-  </si>
-  <si>
     <t>RO</t>
   </si>
   <si>
-    <t>Porto Velho</t>
-  </si>
-  <si>
     <t>RR</t>
   </si>
   <si>
-    <t>Boa Vista</t>
-  </si>
-  <si>
     <t>SC</t>
   </si>
   <si>
-    <t>Florianópolis</t>
-  </si>
-  <si>
     <t>SP</t>
   </si>
   <si>
     <t>SE</t>
   </si>
   <si>
-    <t>Aracaju</t>
-  </si>
-  <si>
     <t>TO</t>
   </si>
   <si>
-    <t>Palmas</t>
-  </si>
-  <si>
     <t>NE</t>
   </si>
   <si>
@@ -312,9 +235,6 @@
   </si>
   <si>
     <t>UF</t>
-  </si>
-  <si>
-    <t>UNIDADES FEDERATIVAS E REGIÕES BRASILEIRAS - SIGLAS</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1044,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -1280,32 +1200,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF808080"/>
       </left>
       <right style="thin">
@@ -1419,17 +1313,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1601,13 +1484,13 @@
     <xf numFmtId="0" fontId="35" fillId="26" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="26" borderId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="41" borderId="15"/>
+    <xf numFmtId="0" fontId="36" fillId="41" borderId="13"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="41" borderId="15"/>
+    <xf numFmtId="0" fontId="36" fillId="41" borderId="13"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="41" borderId="15"/>
+    <xf numFmtId="0" fontId="36" fillId="41" borderId="13"/>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="41" borderId="15"/>
+    <xf numFmtId="0" fontId="36" fillId="41" borderId="13"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -1618,7 +1501,7 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="5"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="5"/>
-    <xf numFmtId="0" fontId="38" fillId="47" borderId="16"/>
+    <xf numFmtId="0" fontId="38" fillId="47" borderId="14"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="38" fillId="47" borderId="3"/>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1660,9 +1543,9 @@
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="45" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="15"/>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="13"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="15"/>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="13"/>
     <xf numFmtId="0" fontId="41" fillId="48" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="43" borderId="0"/>
     <xf numFmtId="0" fontId="42" fillId="48" borderId="0"/>
@@ -1690,16 +1573,16 @@
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="17"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="15"/>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="55" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="18"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="16"/>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="19"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="17"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="19"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="17"/>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -1715,10 +1598,10 @@
     <xf numFmtId="0" fontId="60" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="33" fillId="25" borderId="0"/>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="15"/>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="13"/>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="29" borderId="15"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="20"/>
+    <xf numFmtId="0" fontId="40" fillId="29" borderId="13"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="18"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="5"/>
     <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1854,17 +1737,17 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="50" borderId="21"/>
+    <xf numFmtId="0" fontId="25" fillId="50" borderId="19"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="50" borderId="21"/>
-    <xf numFmtId="0" fontId="70" fillId="50" borderId="15"/>
-    <xf numFmtId="0" fontId="70" fillId="50" borderId="15"/>
+    <xf numFmtId="0" fontId="25" fillId="50" borderId="19"/>
+    <xf numFmtId="0" fontId="70" fillId="50" borderId="13"/>
+    <xf numFmtId="0" fontId="70" fillId="50" borderId="13"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="50" borderId="21"/>
-    <xf numFmtId="0" fontId="71" fillId="50" borderId="15"/>
-    <xf numFmtId="0" fontId="72" fillId="41" borderId="22"/>
+    <xf numFmtId="0" fontId="25" fillId="50" borderId="19"/>
+    <xf numFmtId="0" fontId="71" fillId="50" borderId="13"/>
+    <xf numFmtId="0" fontId="72" fillId="41" borderId="20"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="72" fillId="41" borderId="22"/>
+    <xf numFmtId="0" fontId="72" fillId="41" borderId="20"/>
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="25" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1899,9 +1782,9 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="33" fillId="25" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="72" fillId="41" borderId="22"/>
+    <xf numFmtId="0" fontId="72" fillId="41" borderId="20"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="72" fillId="41" borderId="22"/>
+    <xf numFmtId="0" fontId="72" fillId="41" borderId="20"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="68" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0"/>
@@ -1920,17 +1803,17 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="17"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="15"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="17"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="15"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="18"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="16"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="18"/>
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="16"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="19"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="17"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="19"/>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="17"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1940,12 +1823,12 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="23"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="21"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="23"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="21"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="24"/>
-    <xf numFmtId="0" fontId="76" fillId="0" borderId="23"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="22"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="21"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1977,23 +1860,19 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="74" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="77" fillId="51" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="78" fillId="51" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="533">
@@ -2544,6 +2423,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -2801,516 +2684,402 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304654AF-0E8D-4799-ABB4-2A3D582B96AB}">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{102B2438-C4C2-4BA0-8B4E-C324112E43C4}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:2" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304654AF-0E8D-4799-ABB4-2A3D582B96AB}">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="15">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
+      <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15">
+      <c r="A12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15">
-      <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C15" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15">
+      <c r="A16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15">
+      <c r="A18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15">
+      <c r="A20" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15">
+      <c r="A21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15">
+      <c r="A22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15">
+      <c r="A23" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="15">
-      <c r="A4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15">
-      <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="C23" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15">
+      <c r="A24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15">
+      <c r="A25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15">
+      <c r="A26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15">
+      <c r="A27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="C27" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15">
+      <c r="A28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="15">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="15">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="15">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15">
-      <c r="A13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15">
-      <c r="A14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15">
-      <c r="A16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="15">
-      <c r="A17" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15">
-      <c r="A18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15">
-      <c r="A19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15">
-      <c r="A20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15">
-      <c r="A21" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15">
-      <c r="A22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15">
-      <c r="A23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="15">
-      <c r="A24" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="15">
-      <c r="A25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15">
-      <c r="A26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="15">
-      <c r="A27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15">
-      <c r="A28" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15">
-      <c r="A29" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>90</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:E29" xr:uid="{304654AF-0E8D-4799-ABB4-2A3D582B96AB}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E29">
-      <sortCondition ref="D2:D29"/>
+  <autoFilter ref="A1:C28" xr:uid="{304654AF-0E8D-4799-ABB4-2A3D582B96AB}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C28">
+      <sortCondition ref="C1:C28"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>